<commit_message>
Add brake bias + minor DD updates
</commit_message>
<xml_diff>
--- a/teensy_code/ATCC/TempSensorVoltageCalc.xlsx
+++ b/teensy_code/ATCC/TempSensorVoltageCalc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://michiganstate.sharepoint.com/sites/RSO-MSUFormulaRacingTeam-System-Electrical/Shared Documents/System - Electrical/Electrical_SR22/Data Aq/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveyonkers/Repositories/Electrical-SR20/teensy_code/ATCC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="196" documentId="11_AF1142BE89A88DF71A78F3A52AC4462E5A9198F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A2DCA31-778B-A94E-B6A6-3C77DBC45314}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5164022-8FDB-8048-AB6C-AAC43DA424E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -87,7 +87,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -212,7 +212,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="poly"/>
-            <c:order val="5"/>
+            <c:order val="4"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -1489,7 +1489,7 @@
         <v>57</v>
       </c>
       <c r="C6" s="2">
-        <f>($C$2*B6)/($C$3+B6)</f>
+        <f t="shared" ref="C6:C25" si="0">($C$2*B6)/($C$3+B6)</f>
         <v>0.22673031026252982</v>
       </c>
       <c r="D6" s="1">
@@ -1501,7 +1501,7 @@
         <v>71</v>
       </c>
       <c r="C7" s="2">
-        <f>($C$2*B7)/($C$3+B7)</f>
+        <f t="shared" si="0"/>
         <v>0.27930763178599527</v>
       </c>
       <c r="D7" s="1">
@@ -1513,7 +1513,7 @@
         <v>89</v>
       </c>
       <c r="C8" s="2">
-        <f>($C$2*B8)/($C$3+B8)</f>
+        <f t="shared" si="0"/>
         <v>0.34522885958107058</v>
       </c>
       <c r="D8" s="1">
@@ -1525,7 +1525,7 @@
         <v>113</v>
       </c>
       <c r="C9" s="2">
-        <f>($C$2*B9)/($C$3+B9)</f>
+        <f t="shared" si="0"/>
         <v>0.43031226199543032</v>
       </c>
       <c r="D9" s="1">
@@ -1537,7 +1537,7 @@
         <v>144</v>
       </c>
       <c r="C10" s="2">
-        <f>($C$2*B10)/($C$3+B10)</f>
+        <f t="shared" si="0"/>
         <v>0.5357142857142857</v>
       </c>
       <c r="D10" s="1">
@@ -1549,7 +1549,7 @@
         <v>187</v>
       </c>
       <c r="C11" s="2">
-        <f>($C$2*B11)/($C$3+B11)</f>
+        <f t="shared" si="0"/>
         <v>0.67411679884643116</v>
       </c>
       <c r="D11" s="1">
@@ -1561,7 +1561,7 @@
         <v>243</v>
       </c>
       <c r="C12" s="2">
-        <f>($C$2*B12)/($C$3+B12)</f>
+        <f t="shared" si="0"/>
         <v>0.84199584199584199</v>
       </c>
       <c r="D12" s="1">
@@ -1573,7 +1573,7 @@
         <v>323</v>
       </c>
       <c r="C13" s="2">
-        <f>($C$2*B13)/($C$3+B13)</f>
+        <f t="shared" si="0"/>
         <v>1.0604070912672356</v>
       </c>
       <c r="D13" s="1">
@@ -1585,7 +1585,7 @@
         <v>436</v>
       </c>
       <c r="C14" s="2">
-        <f>($C$2*B14)/($C$3+B14)</f>
+        <f t="shared" si="0"/>
         <v>1.3325183374083129</v>
       </c>
       <c r="D14" s="1">
@@ -1597,7 +1597,7 @@
         <v>596</v>
       </c>
       <c r="C15" s="2">
-        <f>($C$2*B15)/($C$3+B15)</f>
+        <f t="shared" si="0"/>
         <v>1.6592427616926504</v>
       </c>
       <c r="D15" s="1">
@@ -1609,7 +1609,7 @@
         <v>834</v>
       </c>
       <c r="C16" s="2">
-        <f>($C$2*B16)/($C$3+B16)</f>
+        <f t="shared" si="0"/>
         <v>2.0501474926253689</v>
       </c>
       <c r="D16" s="1">
@@ -1621,7 +1621,7 @@
         <v>1175</v>
       </c>
       <c r="C17" s="2">
-        <f>($C$2*B17)/($C$3+B17)</f>
+        <f t="shared" si="0"/>
         <v>2.4736842105263159</v>
       </c>
       <c r="D17" s="1">
@@ -1633,7 +1633,7 @@
         <v>1707</v>
       </c>
       <c r="C18" s="2">
-        <f>($C$2*B18)/($C$3+B18)</f>
+        <f t="shared" si="0"/>
         <v>2.9360165118679049</v>
       </c>
       <c r="D18" s="1">
@@ -1646,7 +1646,7 @@
         <v>2500</v>
       </c>
       <c r="C19" s="2">
-        <f>($C$2*B19)/($C$3+B19)</f>
+        <f t="shared" si="0"/>
         <v>3.3783783783783785</v>
       </c>
       <c r="D19" s="1">
@@ -1659,7 +1659,7 @@
         <v>3792</v>
       </c>
       <c r="C20" s="2">
-        <f>($C$2*B20)/($C$3+B20)</f>
+        <f t="shared" si="0"/>
         <v>3.7980769230769229</v>
       </c>
       <c r="D20" s="1">
@@ -1672,7 +1672,7 @@
         <v>5896</v>
       </c>
       <c r="C21" s="2">
-        <f>($C$2*B21)/($C$3+B21)</f>
+        <f t="shared" si="0"/>
         <v>4.1544532130777903</v>
       </c>
       <c r="D21" s="1">
@@ -1685,7 +1685,7 @@
         <v>9397</v>
       </c>
       <c r="C22" s="2">
-        <f>($C$2*B22)/($C$3+B22)</f>
+        <f t="shared" si="0"/>
         <v>4.4338020194394643</v>
       </c>
       <c r="D22" s="1">
@@ -1698,7 +1698,7 @@
         <v>15462</v>
       </c>
       <c r="C23" s="2">
-        <f>($C$2*B23)/($C$3+B23)</f>
+        <f t="shared" si="0"/>
         <v>4.6398991717680946</v>
       </c>
       <c r="D23" s="1">
@@ -1711,7 +1711,7 @@
         <v>26114</v>
       </c>
       <c r="C24" s="2">
-        <f>($C$2*B24)/($C$3+B24)</f>
+        <f t="shared" si="0"/>
         <v>4.7803324302555463</v>
       </c>
       <c r="D24" s="1">
@@ -1724,7 +1724,7 @@
         <v>45313</v>
       </c>
       <c r="C25" s="2">
-        <f>($C$2*B25)/($C$3+B25)</f>
+        <f t="shared" si="0"/>
         <v>4.8710038053877414</v>
       </c>
       <c r="D25" s="1">
@@ -1784,15 +1784,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100ADD42E1B1C46F143910DFACEDFB3DCD0" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e801ee539fe8b25d1b606feede68dce0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f1a379c5-2064-4021-b960-01be5762b1c0" xmlns:ns3="13e4f39d-d1ea-491c-a2cd-35840b67ca59" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b6518904813d552b46dfe906e10412b" ns2:_="" ns3:_="">
     <xsd:import namespace="f1a379c5-2064-4021-b960-01be5762b1c0"/>
@@ -2009,6 +2000,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8B22DB7-D1F6-478D-8E4A-508B43D995D1}">
   <ds:schemaRefs>
@@ -2027,13 +2027,28 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D34DD5C1-354F-4901-817F-D7B1114830F7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f1a379c5-2064-4021-b960-01be5762b1c0"/>
+    <ds:schemaRef ds:uri="13e4f39d-d1ea-491c-a2cd-35840b67ca59"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19A2747E-AFFD-4AA2-A5ED-204C85F70E33}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D34DD5C1-354F-4901-817F-D7B1114830F7}"/>
 </file>
</xml_diff>